<commit_message>
New format with number of trials
</commit_message>
<xml_diff>
--- a/Data_Bayes.xlsx
+++ b/Data_Bayes.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
+  <si>
+    <t>number of trials</t>
+  </si>
   <si>
     <t>number of parameters</t>
   </si>
@@ -31,40 +34,145 @@
     <t>type_of_opt</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>Trig</t>
-  </si>
-  <si>
-    <t>0.9993723408853696</t>
-  </si>
-  <si>
-    <t>0.998826167853054</t>
-  </si>
-  <si>
-    <t>0.9983483791920693</t>
-  </si>
-  <si>
-    <t>0.9984891372363317</t>
-  </si>
-  <si>
-    <t>0.9993941955409945</t>
-  </si>
-  <si>
-    <t>0.2968326711654663</t>
-  </si>
-  <si>
-    <t>0.21193836688995363</t>
-  </si>
-  <si>
-    <t>0.20650527477264405</t>
-  </si>
-  <si>
-    <t>0.23295145034790038</t>
-  </si>
-  <si>
-    <t>0.2160735034942627</t>
+    <t>trig</t>
+  </si>
+  <si>
+    <t>0.8451595274072212</t>
+  </si>
+  <si>
+    <t>0.8542356998795869</t>
+  </si>
+  <si>
+    <t>1.0001120496197426</t>
+  </si>
+  <si>
+    <t>1.0001201317312995</t>
+  </si>
+  <si>
+    <t>0.9959026419995229</t>
+  </si>
+  <si>
+    <t>0.9994724575240966</t>
+  </si>
+  <si>
+    <t>0.9978737177979694</t>
+  </si>
+  <si>
+    <t>0.99997856635725</t>
+  </si>
+  <si>
+    <t>0.9970316783285063</t>
+  </si>
+  <si>
+    <t>0.998885241735141</t>
+  </si>
+  <si>
+    <t>0.9128775718734097</t>
+  </si>
+  <si>
+    <t>0.9986820565697616</t>
+  </si>
+  <si>
+    <t>0.9990487008470356</t>
+  </si>
+  <si>
+    <t>0.7962357008783424</t>
+  </si>
+  <si>
+    <t>-0.5143707841251646</t>
+  </si>
+  <si>
+    <t>0.9979619874085682</t>
+  </si>
+  <si>
+    <t>0.9997831239942585</t>
+  </si>
+  <si>
+    <t>0.9995893142058129</t>
+  </si>
+  <si>
+    <t>0.040511488914489746</t>
+  </si>
+  <si>
+    <t>0.010579407215118408</t>
+  </si>
+  <si>
+    <t>0.07215124368667603</t>
+  </si>
+  <si>
+    <t>0.04478378295898437</t>
+  </si>
+  <si>
+    <t>0.03006434440612793</t>
+  </si>
+  <si>
+    <t>0.10497495261105624</t>
+  </si>
+  <si>
+    <t>0.06196516752243042</t>
+  </si>
+  <si>
+    <t>0.08458212443760463</t>
+  </si>
+  <si>
+    <t>0.06592309474945068</t>
+  </si>
+  <si>
+    <t>0.06863537430763245</t>
+  </si>
+  <si>
+    <t>0.04181826114654541</t>
+  </si>
+  <si>
+    <t>0.04341447353363037</t>
+  </si>
+  <si>
+    <t>0.040699392557144165</t>
+  </si>
+  <si>
+    <t>0.082881667397239</t>
+  </si>
+  <si>
+    <t>0.022198021411895752</t>
+  </si>
+  <si>
+    <t>0.05018800497055054</t>
+  </si>
+  <si>
+    <t>0.08223039453679865</t>
+  </si>
+  <si>
+    <t>0.07744763578687396</t>
+  </si>
+  <si>
+    <t>0.031387120485305786</t>
   </si>
   <si>
     <t>Bayes</t>
@@ -425,13 +533,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,105 +555,445 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
         <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>